<commit_message>
Corrige extração de horarios de aula
</commit_message>
<xml_diff>
--- a/web/static/dados/planilha_alocacoes.xlsx
+++ b/web/static/dados/planilha_alocacoes.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -70,14 +70,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00ab93f5"/>
-        <bgColor rgb="00ab93f5"/>
+        <fgColor rgb="00ffa500"/>
+        <bgColor rgb="00ff7b59"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00ffa500"/>
-        <bgColor rgb="00ff7b59"/>
+        <fgColor rgb="00ab93f5"/>
+        <bgColor rgb="00ab93f5"/>
       </patternFill>
     </fill>
     <fill>
@@ -224,8 +224,8 @@
     <cellStyle name="estilo_header" xfId="1" hidden="0"/>
     <cellStyle name="estilo_index" xfId="2" hidden="0"/>
     <cellStyle name="separador" xfId="3" hidden="0"/>
-    <cellStyle name="agrupamento" xfId="4" hidden="0"/>
-    <cellStyle name="compartilhamento" xfId="5" hidden="0"/>
+    <cellStyle name="compartilhamento" xfId="4" hidden="0"/>
+    <cellStyle name="agrupamento" xfId="5" hidden="0"/>
     <cellStyle name="fusao" xfId="6" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -826,7 +826,7 @@
       </c>
       <c r="C5" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>EAS - opt (GEN195_1)</t>
         </is>
       </c>
       <c r="D5" s="8" t="inlineStr">
@@ -851,28 +851,28 @@
       </c>
       <c r="H5" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>EAS - opt (GEN204_1)</t>
         </is>
       </c>
       <c r="I5" s="3" t="inlineStr"/>
       <c r="J5" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>EAS - opt (GEN196_1)</t>
         </is>
       </c>
       <c r="K5" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>EAS - opt (GEX458_1)</t>
         </is>
       </c>
       <c r="L5" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>EAS - opt (GCA321_1)</t>
         </is>
       </c>
       <c r="M5" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>EAS - opt (GEN204_1)</t>
         </is>
       </c>
       <c r="N5" s="8" t="inlineStr">
@@ -955,29 +955,29 @@
         </is>
       </c>
       <c r="I6" s="3" t="inlineStr"/>
-      <c r="J6" s="8" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K6" s="8" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L6" s="8" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M6" s="8" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N6" s="8" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="J6" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">EAS - 2 (GEX178_2) | EAS - 2 (GEX607_2) </t>
+        </is>
+      </c>
+      <c r="K6" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">EAS - 2 (GEX186_1) | EAS - 2 (GEX607_2) </t>
+        </is>
+      </c>
+      <c r="L6" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">EAS - 2 (GEX178_2) | EAS - 2 (GEX210_16) </t>
+        </is>
+      </c>
+      <c r="M6" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">EAS - 2 (GCB184_1) | EAS - 2 (GEX186_1) </t>
+        </is>
+      </c>
+      <c r="N6" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">EAS - 2 (GEX206_1) | EAS - 2 (GEX210_16) </t>
         </is>
       </c>
       <c r="O6" s="8" t="inlineStr">
@@ -986,14 +986,14 @@
         </is>
       </c>
       <c r="P6" s="3" t="inlineStr"/>
-      <c r="Q6" s="9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">MAT - 8 (GEX993_1 - GEX994_1) </t>
+      <c r="Q6" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="R6" s="8" t="inlineStr">
         <is>
-          <t>MAT - 2 (GCH293_7)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="S6" s="8" t="inlineStr">
@@ -1003,7 +1003,7 @@
       </c>
       <c r="T6" s="8" t="inlineStr">
         <is>
-          <t>MAT - opt (GEX1000_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U6" s="8" t="inlineStr">
@@ -1026,10 +1026,10 @@
       </c>
       <c r="C7" s="8" t="inlineStr">
         <is>
-          <t>EAS - opt (GEN195_1)</t>
-        </is>
-      </c>
-      <c r="D7" s="10" t="inlineStr">
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D7" s="9" t="inlineStr">
         <is>
           <t xml:space="preserve">EAS - 4 (GCB128_1) | EAS - 4 (GEX219_1) </t>
         </is>
@@ -1051,33 +1051,33 @@
       </c>
       <c r="H7" s="8" t="inlineStr">
         <is>
-          <t>EAS - opt (GEN204_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I7" s="3" t="inlineStr"/>
       <c r="J7" s="8" t="inlineStr">
         <is>
-          <t>EAS - opt (GEN196_1)</t>
+          <t>EAS - 4 (GEX404_1)</t>
         </is>
       </c>
       <c r="K7" s="8" t="inlineStr">
         <is>
-          <t>EAS - 6 (GCA322_1)</t>
-        </is>
-      </c>
-      <c r="L7" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">EAS - 6 (GCA322_1) | EAS - 2 (GEX210_16) </t>
+          <t>EAS - 4 (GEX404_1)</t>
+        </is>
+      </c>
+      <c r="L7" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="M7" s="8" t="inlineStr">
         <is>
-          <t>EAS - opt (GEN204_1)</t>
-        </is>
-      </c>
-      <c r="N7" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">EAS - 2 (GEX206_1) | EAS - 2 (GEX210_16) </t>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N7" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="O7" s="8" t="inlineStr">
@@ -1086,14 +1086,14 @@
         </is>
       </c>
       <c r="P7" s="3" t="inlineStr"/>
-      <c r="Q7" s="8" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="Q7" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MAT - 8 (GEX993_1 - GEX994_1) </t>
         </is>
       </c>
       <c r="R7" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MAT - 2 (GCH293_7)</t>
         </is>
       </c>
       <c r="S7" s="8" t="inlineStr">
@@ -1103,7 +1103,7 @@
       </c>
       <c r="T7" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MAT - opt (GEX1000_1)</t>
         </is>
       </c>
       <c r="U7" s="8" t="inlineStr">
@@ -1131,7 +1131,7 @@
       </c>
       <c r="D8" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>EAS - 6 (GEX298_1)</t>
         </is>
       </c>
       <c r="E8" s="8" t="inlineStr">
@@ -1155,19 +1155,19 @@
         </is>
       </c>
       <c r="I8" s="3" t="inlineStr"/>
-      <c r="J8" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">EAS - 6 (GEX395_2) | EAS - 4 (GEX404_1) </t>
-        </is>
-      </c>
-      <c r="K8" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">EAS - 4 (GEX404_1) | EAS - opt (GEX458_1) </t>
-        </is>
-      </c>
-      <c r="L8" s="8" t="inlineStr">
-        <is>
-          <t>EAS - opt (GCA321_1)</t>
+      <c r="J8" s="8" t="inlineStr">
+        <is>
+          <t>EAS - 6 (GEX395_2)</t>
+        </is>
+      </c>
+      <c r="K8" s="8" t="inlineStr">
+        <is>
+          <t>EAS - 6 (GCA322_1)</t>
+        </is>
+      </c>
+      <c r="L8" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">EAS - 6 (GCA322_1) | EAS - 6 (GEX297_1) </t>
         </is>
       </c>
       <c r="M8" s="8" t="inlineStr">
@@ -1231,7 +1231,7 @@
       </c>
       <c r="D9" s="8" t="inlineStr">
         <is>
-          <t>EAS - 6 (GEX298_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E9" s="8" t="inlineStr">
@@ -1255,24 +1255,24 @@
         </is>
       </c>
       <c r="I9" s="3" t="inlineStr"/>
-      <c r="J9" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">EAS - 2 (GEX178_2) | EAS - 2 (GEX607_2) </t>
-        </is>
-      </c>
-      <c r="K9" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">EAS - 2 (GEX186_1) | EAS - 2 (GEX607_2) </t>
-        </is>
-      </c>
-      <c r="L9" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">EAS - 2 (GEX178_2) | EAS - 6 (GEX297_1) </t>
-        </is>
-      </c>
-      <c r="M9" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">EAS - 2 (GCB184_1) | EAS - 2 (GEX186_1) </t>
+      <c r="J9" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K9" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L9" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M9" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="N9" s="8" t="inlineStr">
@@ -1393,12 +1393,12 @@
       </c>
       <c r="R10" s="8" t="inlineStr">
         <is>
-          <t>LET - 2 (GCH290_14)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="S10" s="8" t="inlineStr">
         <is>
-          <t>LET - 6 (GCH1031_2)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="T10" s="8" t="inlineStr">
@@ -1488,12 +1488,12 @@
       <c r="P11" s="3" t="inlineStr"/>
       <c r="Q11" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>LET - 2 (GCS238_4)</t>
         </is>
       </c>
       <c r="R11" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>LET - 2 (GCH290_14)</t>
         </is>
       </c>
       <c r="S11" s="8" t="inlineStr">
@@ -1503,7 +1503,7 @@
       </c>
       <c r="T11" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>LET - 2 (GCH293_5)</t>
         </is>
       </c>
       <c r="U11" s="8" t="inlineStr">
@@ -1588,7 +1588,7 @@
       <c r="P12" s="3" t="inlineStr"/>
       <c r="Q12" s="8" t="inlineStr">
         <is>
-          <t>LET - 2 (GCS238_4)</t>
+          <t>LET - 8 (GLA391_1)</t>
         </is>
       </c>
       <c r="R12" s="8" t="inlineStr">
@@ -1598,7 +1598,7 @@
       </c>
       <c r="S12" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>LET - 6 (GCH1031_2)</t>
         </is>
       </c>
       <c r="T12" s="8" t="inlineStr">
@@ -1688,7 +1688,7 @@
       <c r="P13" s="3" t="inlineStr"/>
       <c r="Q13" s="8" t="inlineStr">
         <is>
-          <t>LET - 8 (GLA391_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="R13" s="8" t="inlineStr">
@@ -1703,7 +1703,7 @@
       </c>
       <c r="T13" s="8" t="inlineStr">
         <is>
-          <t>LET - 2 (GCH293_5)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U13" s="8" t="inlineStr">
@@ -1831,7 +1831,7 @@
       </c>
       <c r="D15" s="8" t="inlineStr">
         <is>
-          <t>MED - 3 (GSA280_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E15" s="8" t="inlineStr">
@@ -1841,7 +1841,7 @@
       </c>
       <c r="F15" s="8" t="inlineStr">
         <is>
-          <t>MED - 1 (GCH290_13)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G15" s="8" t="inlineStr">
@@ -1855,14 +1855,14 @@
         </is>
       </c>
       <c r="I15" s="3" t="inlineStr"/>
-      <c r="J15" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">MED - 3 (GSA280_1) | MED - opt (GSA299_1) </t>
-        </is>
-      </c>
-      <c r="K15" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">MED - 3 (GSA280_1) | MED - 5 (GSA284_1) </t>
+      <c r="J15" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K15" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="L15" s="8" t="inlineStr">
@@ -1872,12 +1872,12 @@
       </c>
       <c r="M15" s="8" t="inlineStr">
         <is>
-          <t>MED - 5 (GSA283_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="N15" s="8" t="inlineStr">
         <is>
-          <t>MED - 1 (GSA268_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="O15" s="8" t="inlineStr">
@@ -1888,7 +1888,7 @@
       <c r="P15" s="3" t="inlineStr"/>
       <c r="Q15" s="8" t="inlineStr">
         <is>
-          <t>MED - opt (GSA299_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="R15" s="8" t="inlineStr">
@@ -1898,12 +1898,12 @@
       </c>
       <c r="S15" s="8" t="inlineStr">
         <is>
-          <t>MED - opt (GLA192_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="T15" s="8" t="inlineStr">
         <is>
-          <t>MED - 5 (GSA283_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U15" s="8" t="inlineStr">
@@ -1926,27 +1926,27 @@
       </c>
       <c r="C16" s="8" t="inlineStr">
         <is>
-          <t>MED - 1 (GSA271_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D16" s="8" t="inlineStr">
         <is>
-          <t>MED - 1 (GSA271_1)</t>
+          <t>AGRO - opt (GEX431_1)</t>
         </is>
       </c>
       <c r="E16" s="8" t="inlineStr">
         <is>
-          <t>MED - 7 (GSA287_1)</t>
+          <t>AGRO - 8 (GCS073_1)</t>
         </is>
       </c>
       <c r="F16" s="8" t="inlineStr">
         <is>
-          <t>MED - 7 (GCS239_11)</t>
-        </is>
-      </c>
-      <c r="G16" s="8" t="inlineStr">
-        <is>
-          <t>MED - 1 (GSA271_1)</t>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G16" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AGRO - 2 (GEX190_1 - GEX190_2) </t>
         </is>
       </c>
       <c r="H16" s="8" t="inlineStr">
@@ -1957,7 +1957,7 @@
       <c r="I16" s="3" t="inlineStr"/>
       <c r="J16" s="10" t="inlineStr">
         <is>
-          <t xml:space="preserve">MED - 1 (GCH293_8) | MED - 9 (GSA296_1) </t>
+          <t xml:space="preserve">AGRO - 4 (GEX116_1 - GEX116_2) </t>
         </is>
       </c>
       <c r="K16" s="8" t="inlineStr">
@@ -1967,7 +1967,7 @@
       </c>
       <c r="L16" s="8" t="inlineStr">
         <is>
-          <t>MED - 1 (GSA271_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M16" s="8" t="inlineStr">
@@ -1977,7 +1977,7 @@
       </c>
       <c r="N16" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - 2 (GEX179_1)</t>
         </is>
       </c>
       <c r="O16" s="8" t="inlineStr">
@@ -1988,7 +1988,7 @@
       <c r="P16" s="3" t="inlineStr"/>
       <c r="Q16" s="8" t="inlineStr">
         <is>
-          <t>MED - 9 (GSA296_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="R16" s="8" t="inlineStr">
@@ -2003,12 +2003,12 @@
       </c>
       <c r="T16" s="8" t="inlineStr">
         <is>
-          <t>MED - 3 (GSA281_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U16" s="8" t="inlineStr">
         <is>
-          <t>MED - 1 (GLA104_8)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="V16" s="8" t="inlineStr">
@@ -2036,7 +2036,7 @@
       </c>
       <c r="E17" s="8" t="inlineStr">
         <is>
-          <t>AGRO - 8 (GCS073_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F17" s="8" t="inlineStr">
@@ -2044,9 +2044,9 @@
           <t>AGRO - 6 (GEX080_1)</t>
         </is>
       </c>
-      <c r="G17" s="9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">AGRO - 2 (GEX190_1 - GEX190_2) </t>
+      <c r="G17" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="H17" s="8" t="inlineStr">
@@ -2077,7 +2077,7 @@
       </c>
       <c r="N17" s="8" t="inlineStr">
         <is>
-          <t>AGRO - 2 (GEX179_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="O17" s="8" t="inlineStr">
@@ -2086,9 +2086,9 @@
         </is>
       </c>
       <c r="P17" s="3" t="inlineStr"/>
-      <c r="Q17" s="11" t="inlineStr">
-        <is>
-          <t>CS - 8 + HIS - 4 (GCS238_5)</t>
+      <c r="Q17" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CS - 2 (GCH1325_1 - GLA102_1) </t>
         </is>
       </c>
       <c r="R17" s="8" t="inlineStr">
@@ -2096,9 +2096,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="S17" s="8" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="S17" s="11" t="inlineStr">
+        <is>
+          <t>CS - 4 + FIL - 4 + MAT - 4 (GCH838_1)</t>
         </is>
       </c>
       <c r="T17" s="8" t="inlineStr">
@@ -2131,7 +2131,7 @@
       </c>
       <c r="D18" s="8" t="inlineStr">
         <is>
-          <t>AGRO - opt (GEX431_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E18" s="8" t="inlineStr">
@@ -2155,9 +2155,9 @@
         </is>
       </c>
       <c r="I18" s="3" t="inlineStr"/>
-      <c r="J18" s="9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">AGRO - 4 (GEX116_1 - GEX116_2) </t>
+      <c r="J18" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="K18" s="8" t="inlineStr">
@@ -2186,9 +2186,9 @@
         </is>
       </c>
       <c r="P18" s="3" t="inlineStr"/>
-      <c r="Q18" s="9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">CS - 2 (GCH1325_1 - GLA102_1) </t>
+      <c r="Q18" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="R18" s="8" t="inlineStr">
@@ -2196,9 +2196,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="S18" s="11" t="inlineStr">
-        <is>
-          <t>CS - 4 + FIL - 4 + MAT - 4 (GCH838_1)</t>
+      <c r="S18" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="T18" s="8" t="inlineStr">
@@ -2331,7 +2331,7 @@
       </c>
       <c r="D20" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ENF - 10 (GSA049_1)</t>
         </is>
       </c>
       <c r="E20" s="8" t="inlineStr">
@@ -2341,7 +2341,7 @@
       </c>
       <c r="F20" s="8" t="inlineStr">
         <is>
-          <t>HIS - 8 (GCH390_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G20" s="8" t="inlineStr">
@@ -2357,27 +2357,27 @@
       <c r="I20" s="3" t="inlineStr"/>
       <c r="J20" s="8" t="inlineStr">
         <is>
-          <t>ENF - 2 (GCB064_1)</t>
+          <t>ENF - 10 (GSA047_1)</t>
         </is>
       </c>
       <c r="K20" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ENF - 10 (GSA047_1)</t>
         </is>
       </c>
       <c r="L20" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ENF - 10 (GSA047_1)</t>
         </is>
       </c>
       <c r="M20" s="8" t="inlineStr">
         <is>
-          <t>ENF - 4 (GCB029_1)</t>
+          <t>ENF - 10 (GSA047_1)</t>
         </is>
       </c>
       <c r="N20" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ENF - 10 (GSA047_1)</t>
         </is>
       </c>
       <c r="O20" s="8" t="inlineStr">
@@ -2386,29 +2386,29 @@
         </is>
       </c>
       <c r="P20" s="3" t="inlineStr"/>
-      <c r="Q20" s="8" t="inlineStr">
-        <is>
-          <t>HIS - 2 (GCH290_15)</t>
+      <c r="Q20" s="11" t="inlineStr">
+        <is>
+          <t>CS - 8 + HIS - 4 (GCS238_5)</t>
         </is>
       </c>
       <c r="R20" s="8" t="inlineStr">
         <is>
-          <t>HIS - 2 (GCH291_3)</t>
-        </is>
-      </c>
-      <c r="S20" s="9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">HIS - opt (GCH459_1 - GCH467_1) </t>
+          <t>HIS - 7 (GLA108_1)</t>
+        </is>
+      </c>
+      <c r="S20" s="8" t="inlineStr">
+        <is>
+          <t>HIS - opt (GCH467_1)</t>
         </is>
       </c>
       <c r="T20" s="8" t="inlineStr">
         <is>
-          <t>HIS - 8 (GCH390_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U20" s="8" t="inlineStr">
         <is>
-          <t>HIS - 8 (GCH388_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="V20" s="8" t="inlineStr">
@@ -2426,7 +2426,7 @@
       </c>
       <c r="C21" s="8" t="inlineStr">
         <is>
-          <t>ENF - 4 (GCB064_2)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D21" s="8" t="inlineStr">
@@ -2441,7 +2441,7 @@
       </c>
       <c r="F21" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>HIS - 8 (GCH390_1)</t>
         </is>
       </c>
       <c r="G21" s="8" t="inlineStr">
@@ -2462,7 +2462,7 @@
       </c>
       <c r="K21" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ENF - 6 (GSA044_1)</t>
         </is>
       </c>
       <c r="L21" s="8" t="inlineStr">
@@ -2472,12 +2472,12 @@
       </c>
       <c r="M21" s="8" t="inlineStr">
         <is>
-          <t>ENF - 2 (GCB019_1)</t>
+          <t>ENF - 6 (GSA044_1)</t>
         </is>
       </c>
       <c r="N21" s="8" t="inlineStr">
         <is>
-          <t>ENF - 4 (GCB019_2)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="O21" s="8" t="inlineStr">
@@ -2493,22 +2493,22 @@
       </c>
       <c r="R21" s="8" t="inlineStr">
         <is>
-          <t>HIS - 7 (GLA108_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="S21" s="8" t="inlineStr">
         <is>
-          <t>HIS - 2 (GCH366_1)</t>
+          <t>HIS - opt (GCH459_1)</t>
         </is>
       </c>
       <c r="T21" s="8" t="inlineStr">
         <is>
-          <t>HIS - 2 (GCH365_1)</t>
+          <t>HIS - 8 (GCH390_1)</t>
         </is>
       </c>
       <c r="U21" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>HIS - 8 (GCH388_1)</t>
         </is>
       </c>
       <c r="V21" s="8" t="inlineStr">
@@ -2531,17 +2531,17 @@
       </c>
       <c r="D22" s="8" t="inlineStr">
         <is>
-          <t>ENF - 10 (GSA049_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E22" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ENF - 2 (GSA0304_1)</t>
         </is>
       </c>
       <c r="F22" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ENF - 2 (GSA0305_1)</t>
         </is>
       </c>
       <c r="G22" s="8" t="inlineStr">
@@ -2557,27 +2557,27 @@
       <c r="I22" s="3" t="inlineStr"/>
       <c r="J22" s="8" t="inlineStr">
         <is>
-          <t>ENF - 10 (GSA047_1)</t>
+          <t>ENF - 2 (GCB064_1)</t>
         </is>
       </c>
       <c r="K22" s="8" t="inlineStr">
         <is>
-          <t>ENF - 10 (GSA047_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="L22" s="8" t="inlineStr">
         <is>
-          <t>ENF - 10 (GSA047_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M22" s="8" t="inlineStr">
         <is>
-          <t>ENF - 10 (GSA047_1)</t>
+          <t>ENF - 2 (GCB019_1)</t>
         </is>
       </c>
       <c r="N22" s="8" t="inlineStr">
         <is>
-          <t>ENF - 10 (GSA047_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="O22" s="8" t="inlineStr">
@@ -2588,22 +2588,22 @@
       <c r="P22" s="3" t="inlineStr"/>
       <c r="Q22" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>HIS - 2 (GCH290_15)</t>
         </is>
       </c>
       <c r="R22" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>HIS - 2 (GCH291_3)</t>
         </is>
       </c>
       <c r="S22" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>HIS - 2 (GCH366_1)</t>
         </is>
       </c>
       <c r="T22" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>HIS - 2 (GCH365_1)</t>
         </is>
       </c>
       <c r="U22" s="8" t="inlineStr">
@@ -2626,7 +2626,7 @@
       </c>
       <c r="C23" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ENF - 4 (GCB064_2)</t>
         </is>
       </c>
       <c r="D23" s="8" t="inlineStr">
@@ -2636,12 +2636,12 @@
       </c>
       <c r="E23" s="8" t="inlineStr">
         <is>
-          <t>ENF - 2 (GSA0304_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F23" s="8" t="inlineStr">
         <is>
-          <t>ENF - 2 (GSA0305_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G23" s="8" t="inlineStr">
@@ -2662,7 +2662,7 @@
       </c>
       <c r="K23" s="8" t="inlineStr">
         <is>
-          <t>ENF - 6 (GSA044_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="L23" s="8" t="inlineStr">
@@ -2672,12 +2672,12 @@
       </c>
       <c r="M23" s="8" t="inlineStr">
         <is>
-          <t>ENF - 6 (GSA044_1)</t>
+          <t>ENF - 4 (GCB029_1)</t>
         </is>
       </c>
       <c r="N23" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ENF - 4 (GCB019_2)</t>
         </is>
       </c>
       <c r="O23" s="8" t="inlineStr">
@@ -3154,17 +3154,17 @@
       </c>
       <c r="C29" s="8" t="inlineStr">
         <is>
-          <t>PED - 6 (GLA239_1)</t>
-        </is>
-      </c>
-      <c r="D29" s="9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">PED - 2 (GCH1038_1 - GCH1039_1) </t>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D29" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="E29" s="8" t="inlineStr">
         <is>
-          <t>PED - 2 (GCH1037_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F29" s="8" t="inlineStr">
@@ -3216,27 +3216,27 @@
       <c r="P29" s="3" t="inlineStr"/>
       <c r="Q29" s="8" t="inlineStr">
         <is>
-          <t>PED - 5 (GLA237_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="R29" s="8" t="inlineStr">
         <is>
-          <t>PED - 3 (GCH1087_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="S29" s="8" t="inlineStr">
         <is>
-          <t>PED - opt (GCH1301_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="T29" s="8" t="inlineStr">
         <is>
-          <t>PED - 7 (GLA240_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U29" s="8" t="inlineStr">
         <is>
-          <t>PED - opt (GCH1284_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="V29" s="8" t="inlineStr">
@@ -3264,7 +3264,7 @@
       </c>
       <c r="E30" s="8" t="inlineStr">
         <is>
-          <t>PED - 6 (GLA238_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F30" s="8" t="inlineStr">
@@ -3316,7 +3316,7 @@
       <c r="P30" s="3" t="inlineStr"/>
       <c r="Q30" s="8" t="inlineStr">
         <is>
-          <t>PED - 3 (GCH1086_1)</t>
+          <t>PED - 1 (GCH1036_1)</t>
         </is>
       </c>
       <c r="R30" s="8" t="inlineStr">
@@ -3336,7 +3336,7 @@
       </c>
       <c r="U30" s="8" t="inlineStr">
         <is>
-          <t>PED - 3 (GCH1088_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="V30" s="8" t="inlineStr">
@@ -3354,7 +3354,7 @@
       </c>
       <c r="C31" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>PED - 6 (GLA239_1)</t>
         </is>
       </c>
       <c r="D31" s="8" t="inlineStr">
@@ -3364,7 +3364,7 @@
       </c>
       <c r="E31" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>PED - 6 (GLA238_1)</t>
         </is>
       </c>
       <c r="F31" s="8" t="inlineStr">
@@ -3416,12 +3416,12 @@
       <c r="P31" s="3" t="inlineStr"/>
       <c r="Q31" s="8" t="inlineStr">
         <is>
-          <t>PED - 1 (GCH1036_1)</t>
+          <t>PED - 3 (GCH1086_1)</t>
         </is>
       </c>
       <c r="R31" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>PED - 3 (GCH1087_1)</t>
         </is>
       </c>
       <c r="S31" s="8" t="inlineStr">
@@ -3431,12 +3431,12 @@
       </c>
       <c r="T31" s="8" t="inlineStr">
         <is>
-          <t>PED - opt (GCH1286_1)</t>
+          <t>PED - 9 (GCH1280_1)</t>
         </is>
       </c>
       <c r="U31" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>PED - 3 (GCH1088_1)</t>
         </is>
       </c>
       <c r="V31" s="8" t="inlineStr">
@@ -3516,7 +3516,7 @@
       <c r="P32" s="3" t="inlineStr"/>
       <c r="Q32" s="8" t="inlineStr">
         <is>
-          <t>PED - 7 (GLA213_1)</t>
+          <t>PED - 5 (GLA237_1)</t>
         </is>
       </c>
       <c r="R32" s="8" t="inlineStr">
@@ -3526,17 +3526,17 @@
       </c>
       <c r="S32" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>PED - opt (GCH1301_1)</t>
         </is>
       </c>
       <c r="T32" s="8" t="inlineStr">
         <is>
-          <t>PED - 9 (GCH1280_1)</t>
+          <t>PED - opt (GCH1286_1)</t>
         </is>
       </c>
       <c r="U32" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>PED - opt (GCH1284_1)</t>
         </is>
       </c>
       <c r="V32" s="8" t="inlineStr">
@@ -3557,14 +3557,14 @@
           <t>-</t>
         </is>
       </c>
-      <c r="D33" s="8" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="D33" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PED - 2 (GCH1038_1 - GCH1039_1) </t>
         </is>
       </c>
       <c r="E33" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>PED - 2 (GCH1037_1)</t>
         </is>
       </c>
       <c r="F33" s="8" t="inlineStr">
@@ -3616,7 +3616,7 @@
       <c r="P33" s="3" t="inlineStr"/>
       <c r="Q33" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>PED - 7 (GLA213_1)</t>
         </is>
       </c>
       <c r="R33" s="8" t="inlineStr">
@@ -3631,7 +3631,7 @@
       </c>
       <c r="T33" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>PED - 7 (GLA240_1)</t>
         </is>
       </c>
       <c r="U33" s="8" t="inlineStr">
@@ -3659,12 +3659,12 @@
       </c>
       <c r="D34" s="8" t="inlineStr">
         <is>
-          <t>ADM - 8 (GCS546_1)</t>
+          <t>ADM - 6 (GCS541_1)</t>
         </is>
       </c>
       <c r="E34" s="8" t="inlineStr">
         <is>
-          <t>ADM - 8 (GCS548_1)</t>
+          <t>ADM - 6 (GCS543_1)</t>
         </is>
       </c>
       <c r="F34" s="8" t="inlineStr">
@@ -3721,7 +3721,7 @@
       </c>
       <c r="R34" s="8" t="inlineStr">
         <is>
-          <t>ADM - 9 (GCS549_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="S34" s="8" t="inlineStr">
@@ -3759,12 +3759,12 @@
       </c>
       <c r="D35" s="8" t="inlineStr">
         <is>
-          <t>ADM - 6 (GCS541_1)</t>
+          <t>ADM - 8 (GCS546_1)</t>
         </is>
       </c>
       <c r="E35" s="8" t="inlineStr">
         <is>
-          <t>ADM - 6 (GCS543_1)</t>
+          <t>ADM - 8 (GCS548_1)</t>
         </is>
       </c>
       <c r="F35" s="8" t="inlineStr">
@@ -3821,7 +3821,7 @@
       </c>
       <c r="R35" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ADM - 9 (GCS549_1)</t>
         </is>
       </c>
       <c r="S35" s="8" t="inlineStr">
@@ -4254,12 +4254,12 @@
       </c>
       <c r="C40" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MED - 1 (GSA271_1)</t>
         </is>
       </c>
       <c r="D40" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MED - 1 (GSA271_1)</t>
         </is>
       </c>
       <c r="E40" s="8" t="inlineStr">
@@ -4269,12 +4269,12 @@
       </c>
       <c r="F40" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MED - 1 (GCH290_13)</t>
         </is>
       </c>
       <c r="G40" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MED - 1 (GSA271_1)</t>
         </is>
       </c>
       <c r="H40" s="8" t="inlineStr">
@@ -4283,29 +4283,29 @@
         </is>
       </c>
       <c r="I40" s="3" t="inlineStr"/>
-      <c r="J40" s="8" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="J40" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MED - 1 (GCH293_8) | MED - opt (GSA299_1) </t>
         </is>
       </c>
       <c r="K40" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MED - 5 (GSA284_1)</t>
         </is>
       </c>
       <c r="L40" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MED - 1 (GSA271_1)</t>
         </is>
       </c>
       <c r="M40" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MED - 5 (GSA283_1)</t>
         </is>
       </c>
       <c r="N40" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MED - 1 (GSA268_1)</t>
         </is>
       </c>
       <c r="O40" s="8" t="inlineStr">
@@ -4316,7 +4316,7 @@
       <c r="P40" s="3" t="inlineStr"/>
       <c r="Q40" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MED - opt (GSA299_1)</t>
         </is>
       </c>
       <c r="R40" s="8" t="inlineStr">
@@ -4326,17 +4326,17 @@
       </c>
       <c r="S40" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MED - opt (GLA192_1)</t>
         </is>
       </c>
       <c r="T40" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MED - 5 (GSA283_1)</t>
         </is>
       </c>
       <c r="U40" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MED - 1 (GLA104_8)</t>
         </is>
       </c>
       <c r="V40" s="8" t="inlineStr">
@@ -4359,17 +4359,17 @@
       </c>
       <c r="D41" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MED - 3 (GSA280_1)</t>
         </is>
       </c>
       <c r="E41" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MED - 7 (GSA287_1)</t>
         </is>
       </c>
       <c r="F41" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MED - 7 (GCS239_11)</t>
         </is>
       </c>
       <c r="G41" s="8" t="inlineStr">
@@ -4383,14 +4383,14 @@
         </is>
       </c>
       <c r="I41" s="3" t="inlineStr"/>
-      <c r="J41" s="8" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="J41" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MED - 3 (GSA280_1) | MED - 9 (GSA296_1) </t>
         </is>
       </c>
       <c r="K41" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MED - 3 (GSA280_1)</t>
         </is>
       </c>
       <c r="L41" s="8" t="inlineStr">
@@ -4416,7 +4416,7 @@
       <c r="P41" s="3" t="inlineStr"/>
       <c r="Q41" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MED - 9 (GSA296_1)</t>
         </is>
       </c>
       <c r="R41" s="8" t="inlineStr">
@@ -4431,7 +4431,7 @@
       </c>
       <c r="T41" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MED - 3 (GSA281_1)</t>
         </is>
       </c>
       <c r="U41" s="8" t="inlineStr">
@@ -4469,43 +4469,43 @@
       </c>
       <c r="F42" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>CC - 8 (GEX658_1)</t>
         </is>
       </c>
       <c r="G42" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>CC - 8 (GEX658_1)</t>
         </is>
       </c>
       <c r="H42" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>CC - 8 (GEX658_1)</t>
         </is>
       </c>
       <c r="I42" s="3" t="inlineStr"/>
       <c r="J42" s="8" t="inlineStr">
         <is>
-          <t>CC - 4 (GEX613_2)</t>
-        </is>
-      </c>
-      <c r="K42" s="8" t="inlineStr">
+          <t>CC - 8 (GCS239_2)</t>
+        </is>
+      </c>
+      <c r="K42" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CC - 6 (GCS580_1) | CC - 6 (GEX614_1) </t>
+        </is>
+      </c>
+      <c r="L42" s="8" t="inlineStr">
+        <is>
+          <t>CC - 6 (GCH292_2)</t>
+        </is>
+      </c>
+      <c r="M42" s="8" t="inlineStr">
         <is>
           <t>CC - 6 (GCS580_1)</t>
         </is>
       </c>
-      <c r="L42" s="8" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M42" s="8" t="inlineStr">
-        <is>
-          <t>CC - 6 (GCS580_1)</t>
-        </is>
-      </c>
       <c r="N42" s="8" t="inlineStr">
         <is>
-          <t>CC - 4 (GEX613_2)</t>
+          <t>CC - 6 (GEX614_1)</t>
         </is>
       </c>
       <c r="O42" s="8" t="inlineStr">
@@ -4526,17 +4526,17 @@
       </c>
       <c r="S42" s="8" t="inlineStr">
         <is>
-          <t>CC - 4 (GCH290_5)</t>
+          <t>CC - 7 (GEX618_1)</t>
         </is>
       </c>
       <c r="T42" s="8" t="inlineStr">
         <is>
-          <t>CC - 1 (GEX003_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U42" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>CC - 7 (GEX617_1)</t>
         </is>
       </c>
       <c r="V42" s="8" t="inlineStr">
@@ -4569,17 +4569,17 @@
       </c>
       <c r="F43" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>CC - 9 (GEX657_1)</t>
         </is>
       </c>
       <c r="G43" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>CC - 9 (GEX657_1)</t>
         </is>
       </c>
       <c r="H43" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>CC - 9 (GEX657_1)</t>
         </is>
       </c>
       <c r="I43" s="3" t="inlineStr"/>
@@ -4616,7 +4616,7 @@
       <c r="P43" s="3" t="inlineStr"/>
       <c r="Q43" s="8" t="inlineStr">
         <is>
-          <t>CC - 1 (GCH293_2)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="R43" s="8" t="inlineStr">
@@ -4626,7 +4626,7 @@
       </c>
       <c r="S43" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>CC - 4 (GCH290_5)</t>
         </is>
       </c>
       <c r="T43" s="8" t="inlineStr">
@@ -4636,7 +4636,7 @@
       </c>
       <c r="U43" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>CC - 5 (GEX616_1)</t>
         </is>
       </c>
       <c r="V43" s="8" t="inlineStr">
@@ -4669,28 +4669,28 @@
       </c>
       <c r="F44" s="8" t="inlineStr">
         <is>
-          <t>CC - 8 (GEX658_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G44" s="8" t="inlineStr">
         <is>
-          <t>CC - 8 (GEX658_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H44" s="8" t="inlineStr">
         <is>
-          <t>CC - 8 (GEX658_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I44" s="3" t="inlineStr"/>
       <c r="J44" s="8" t="inlineStr">
         <is>
-          <t>CC - 8 (GCS239_2)</t>
-        </is>
-      </c>
-      <c r="K44" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">CC - 4 (GEN254_1) | CC - 6 (GEX614_1) </t>
+          <t>CC - 4 (GEX613_2)</t>
+        </is>
+      </c>
+      <c r="K44" s="8" t="inlineStr">
+        <is>
+          <t>CC - 4 (GEN254_1)</t>
         </is>
       </c>
       <c r="L44" s="8" t="inlineStr">
@@ -4703,9 +4703,9 @@
           <t>CC - 4 (GEN254_1)</t>
         </is>
       </c>
-      <c r="N44" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">CC - 4 (GEX090_1) | CC - 6 (GEX614_1) </t>
+      <c r="N44" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CC - 4 (GEX090_1) | CC - 4 (GEX613_2) </t>
         </is>
       </c>
       <c r="O44" s="8" t="inlineStr">
@@ -4726,7 +4726,7 @@
       </c>
       <c r="S44" s="8" t="inlineStr">
         <is>
-          <t>CC - 2 (GLA104_2)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="T44" s="8" t="inlineStr">
@@ -4736,7 +4736,7 @@
       </c>
       <c r="U44" s="8" t="inlineStr">
         <is>
-          <t>CC - 7 (GEX617_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="V44" s="8" t="inlineStr">
@@ -4769,17 +4769,17 @@
       </c>
       <c r="F45" s="8" t="inlineStr">
         <is>
-          <t>CC - 9 (GEX657_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G45" s="8" t="inlineStr">
         <is>
-          <t>CC - 9 (GEX657_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H45" s="8" t="inlineStr">
         <is>
-          <t>CC - 9 (GEX657_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I45" s="3" t="inlineStr"/>
@@ -4795,7 +4795,7 @@
       </c>
       <c r="L45" s="8" t="inlineStr">
         <is>
-          <t>CC - 6 (GCH292_2)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M45" s="8" t="inlineStr">
@@ -4816,7 +4816,7 @@
       <c r="P45" s="3" t="inlineStr"/>
       <c r="Q45" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>CC - 1 (GCH293_2)</t>
         </is>
       </c>
       <c r="R45" s="8" t="inlineStr">
@@ -4826,17 +4826,17 @@
       </c>
       <c r="S45" s="8" t="inlineStr">
         <is>
-          <t>CC - 7 (GEX618_1)</t>
+          <t>CC - 2 (GLA104_2)</t>
         </is>
       </c>
       <c r="T45" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>CC - 1 (GEX003_1)</t>
         </is>
       </c>
       <c r="U45" s="8" t="inlineStr">
         <is>
-          <t>CC - 5 (GEX616_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="V45" s="8" t="inlineStr">
@@ -5318,7 +5318,7 @@
       </c>
       <c r="K51" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>FIL - 6 (GCH837_1)</t>
         </is>
       </c>
       <c r="L51" s="8" t="inlineStr">
@@ -5328,7 +5328,7 @@
       </c>
       <c r="M51" s="8" t="inlineStr">
         <is>
-          <t>FIL - 2 (GCH845_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="N51" s="8" t="inlineStr">
@@ -5338,28 +5338,28 @@
       </c>
       <c r="O51" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>FIL - 8 (GCH843_1)</t>
         </is>
       </c>
       <c r="P51" s="3" t="inlineStr"/>
       <c r="Q51" s="8" t="inlineStr">
         <is>
-          <t>FIL - 4 (GCH847_1)</t>
+          <t>FIL - 6 (GCH839_2)</t>
         </is>
       </c>
       <c r="R51" s="8" t="inlineStr">
         <is>
-          <t>FIL - 2 (GLA103_3)</t>
+          <t>FIL - 6 (GCH837_1)</t>
         </is>
       </c>
       <c r="S51" s="8" t="inlineStr">
         <is>
-          <t>FIL - 2 (GEX211_2)</t>
+          <t>FIL - 8 (GCH844_1)</t>
         </is>
       </c>
       <c r="T51" s="8" t="inlineStr">
         <is>
-          <t>FIL - 2 (GCH845_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U51" s="8" t="inlineStr">
@@ -5418,7 +5418,7 @@
       </c>
       <c r="K52" s="8" t="inlineStr">
         <is>
-          <t>FIL - 6 (GCH837_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="L52" s="8" t="inlineStr">
@@ -5428,7 +5428,7 @@
       </c>
       <c r="M52" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>FIL - 2 (GCH845_1)</t>
         </is>
       </c>
       <c r="N52" s="8" t="inlineStr">
@@ -5438,28 +5438,28 @@
       </c>
       <c r="O52" s="8" t="inlineStr">
         <is>
-          <t>FIL - 8 (GCH843_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="P52" s="3" t="inlineStr"/>
       <c r="Q52" s="8" t="inlineStr">
         <is>
-          <t>FIL - 6 (GCH839_2)</t>
+          <t>FIL - 4 (GCH847_1)</t>
         </is>
       </c>
       <c r="R52" s="8" t="inlineStr">
         <is>
-          <t>FIL - 6 (GCH837_1)</t>
+          <t>FIL - 2 (GLA103_3)</t>
         </is>
       </c>
       <c r="S52" s="8" t="inlineStr">
         <is>
-          <t>FIL - 8 (GCH844_1)</t>
+          <t>FIL - 2 (GEX211_2)</t>
         </is>
       </c>
       <c r="T52" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>FIL - 2 (GCH845_1)</t>
         </is>
       </c>
       <c r="U52" s="8" t="inlineStr">

</xml_diff>

<commit_message>
Atualiza interface web para utilizar funcionlidades mais recentes do alocador
</commit_message>
<xml_diff>
--- a/web/static/dados/planilha_alocacoes.xlsx
+++ b/web/static/dados/planilha_alocacoes.xlsx
@@ -46,7 +46,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill/>
     </fill>
@@ -78,12 +78,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="00ab93f5"/>
         <bgColor rgb="00ab93f5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00ff7b59"/>
-        <bgColor rgb="00ff7b59"/>
       </patternFill>
     </fill>
   </fills>
@@ -165,7 +159,7 @@
       </bottom>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -182,11 +176,8 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="9" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -214,19 +205,15 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="5">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="6">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
     <cellStyle name="estilo_header" xfId="1" hidden="0"/>
     <cellStyle name="estilo_index" xfId="2" hidden="0"/>
     <cellStyle name="separador" xfId="3" hidden="0"/>
     <cellStyle name="compartilhamento" xfId="4" hidden="0"/>
     <cellStyle name="agrupamento" xfId="5" hidden="0"/>
-    <cellStyle name="fusao" xfId="6" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -826,7 +813,7 @@
       </c>
       <c r="C5" s="8" t="inlineStr">
         <is>
-          <t>EAS - opt (GEN195_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D5" s="8" t="inlineStr">
@@ -851,28 +838,28 @@
       </c>
       <c r="H5" s="8" t="inlineStr">
         <is>
-          <t>EAS - opt (GEN204_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I5" s="3" t="inlineStr"/>
       <c r="J5" s="8" t="inlineStr">
         <is>
-          <t>EAS - opt (GEN196_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="K5" s="8" t="inlineStr">
         <is>
-          <t>EAS - opt (GEX458_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="L5" s="8" t="inlineStr">
         <is>
-          <t>EAS - opt (GCA321_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M5" s="8" t="inlineStr">
         <is>
-          <t>EAS - opt (GEN204_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="N5" s="8" t="inlineStr">
@@ -955,29 +942,29 @@
         </is>
       </c>
       <c r="I6" s="3" t="inlineStr"/>
-      <c r="J6" s="9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">EAS - 2 (GEX178_2) | EAS - 2 (GEX607_2) </t>
-        </is>
-      </c>
-      <c r="K6" s="9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">EAS - 2 (GEX186_1) | EAS - 2 (GEX607_2) </t>
-        </is>
-      </c>
-      <c r="L6" s="9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">EAS - 2 (GEX178_2) | EAS - 2 (GEX210_16) </t>
-        </is>
-      </c>
-      <c r="M6" s="9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">EAS - 2 (GCB184_1) | EAS - 2 (GEX186_1) </t>
-        </is>
-      </c>
-      <c r="N6" s="9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">EAS - 2 (GEX206_1) | EAS - 2 (GEX210_16) </t>
+      <c r="J6" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K6" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L6" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M6" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N6" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="O6" s="8" t="inlineStr">
@@ -988,7 +975,7 @@
       <c r="P6" s="3" t="inlineStr"/>
       <c r="Q6" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MAT - 1 (GEX213_1)</t>
         </is>
       </c>
       <c r="R6" s="8" t="inlineStr">
@@ -998,7 +985,7 @@
       </c>
       <c r="S6" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MAT - 1 (GLA104_1)</t>
         </is>
       </c>
       <c r="T6" s="8" t="inlineStr">
@@ -1029,24 +1016,24 @@
           <t>-</t>
         </is>
       </c>
-      <c r="D7" s="9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">EAS - 4 (GCB128_1) | EAS - 4 (GEX219_1) </t>
+      <c r="D7" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="E7" s="8" t="inlineStr">
         <is>
-          <t>EAS - 4 (GEX296_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F7" s="8" t="inlineStr">
         <is>
-          <t>EAS - 4 (GEX067_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G7" s="8" t="inlineStr">
         <is>
-          <t>EAS - 4 (GEX219_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H7" s="8" t="inlineStr">
@@ -1057,12 +1044,12 @@
       <c r="I7" s="3" t="inlineStr"/>
       <c r="J7" s="8" t="inlineStr">
         <is>
-          <t>EAS - 4 (GEX404_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="K7" s="8" t="inlineStr">
         <is>
-          <t>EAS - 4 (GEX404_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="L7" s="8" t="inlineStr">
@@ -1086,14 +1073,14 @@
         </is>
       </c>
       <c r="P7" s="3" t="inlineStr"/>
-      <c r="Q7" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">MAT - 8 (GEX993_1 - GEX994_1) </t>
+      <c r="Q7" s="8" t="inlineStr">
+        <is>
+          <t>MAT - 3 (GEX969_1)</t>
         </is>
       </c>
       <c r="R7" s="8" t="inlineStr">
         <is>
-          <t>MAT - 2 (GCH293_7)</t>
+          <t>MAT - 3 (GEX968_1)</t>
         </is>
       </c>
       <c r="S7" s="8" t="inlineStr">
@@ -1103,12 +1090,12 @@
       </c>
       <c r="T7" s="8" t="inlineStr">
         <is>
-          <t>MAT - opt (GEX1000_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U7" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MAT - 3 (GCH839_1)</t>
         </is>
       </c>
       <c r="V7" s="8" t="inlineStr">
@@ -1131,7 +1118,7 @@
       </c>
       <c r="D8" s="8" t="inlineStr">
         <is>
-          <t>EAS - 6 (GEX298_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E8" s="8" t="inlineStr">
@@ -1157,22 +1144,22 @@
       <c r="I8" s="3" t="inlineStr"/>
       <c r="J8" s="8" t="inlineStr">
         <is>
-          <t>EAS - 6 (GEX395_2)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="K8" s="8" t="inlineStr">
         <is>
-          <t>EAS - 6 (GCA322_1)</t>
-        </is>
-      </c>
-      <c r="L8" s="9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">EAS - 6 (GCA322_1) | EAS - 6 (GEX297_1) </t>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L8" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="M8" s="8" t="inlineStr">
         <is>
-          <t>EAS - 6 (GEX395_2)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="N8" s="8" t="inlineStr">
@@ -1224,9 +1211,9 @@
           <t>205-A</t>
         </is>
       </c>
-      <c r="C9" s="8" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="C9" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">EAS - opt (GEN198_1) | EAS - opt (GEN199_1) </t>
         </is>
       </c>
       <c r="D9" s="8" t="inlineStr">
@@ -1246,7 +1233,7 @@
       </c>
       <c r="G9" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>EAS - opt (GEN200_1)</t>
         </is>
       </c>
       <c r="H9" s="8" t="inlineStr">
@@ -1257,7 +1244,7 @@
       <c r="I9" s="3" t="inlineStr"/>
       <c r="J9" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>EAS - opt (GEN193_1)</t>
         </is>
       </c>
       <c r="K9" s="8" t="inlineStr">
@@ -1357,27 +1344,27 @@
       <c r="I10" s="3" t="inlineStr"/>
       <c r="J10" s="8" t="inlineStr">
         <is>
-          <t>LET - opt (GLA552_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="K10" s="8" t="inlineStr">
         <is>
-          <t>LET - opt (GLA552_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="L10" s="8" t="inlineStr">
         <is>
-          <t>LET - opt (GLA552_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M10" s="8" t="inlineStr">
         <is>
-          <t>LET - opt (GLA552_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="N10" s="8" t="inlineStr">
         <is>
-          <t>LET - opt (GLA552_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="O10" s="8" t="inlineStr">
@@ -1403,7 +1390,7 @@
       </c>
       <c r="T10" s="8" t="inlineStr">
         <is>
-          <t>LET - opt (GLA528_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U10" s="8" t="inlineStr">
@@ -1488,12 +1475,12 @@
       <c r="P11" s="3" t="inlineStr"/>
       <c r="Q11" s="8" t="inlineStr">
         <is>
-          <t>LET - 2 (GCS238_4)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="R11" s="8" t="inlineStr">
         <is>
-          <t>LET - 2 (GCH290_14)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="S11" s="8" t="inlineStr">
@@ -1503,7 +1490,7 @@
       </c>
       <c r="T11" s="8" t="inlineStr">
         <is>
-          <t>LET - 2 (GCH293_5)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U11" s="8" t="inlineStr">
@@ -1588,7 +1575,7 @@
       <c r="P12" s="3" t="inlineStr"/>
       <c r="Q12" s="8" t="inlineStr">
         <is>
-          <t>LET - 8 (GLA391_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="R12" s="8" t="inlineStr">
@@ -1598,12 +1585,12 @@
       </c>
       <c r="S12" s="8" t="inlineStr">
         <is>
-          <t>LET - 6 (GCH1031_2)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="T12" s="8" t="inlineStr">
         <is>
-          <t>LET - 8 (GLA392_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U12" s="8" t="inlineStr">
@@ -1826,43 +1813,43 @@
       </c>
       <c r="C15" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - 9 (GCS085_1)</t>
         </is>
       </c>
       <c r="D15" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - 9 (GCA060_1)</t>
         </is>
       </c>
       <c r="E15" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - 9 (GCA268_1)</t>
         </is>
       </c>
       <c r="F15" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - 9 (GCA057_1)</t>
         </is>
       </c>
       <c r="G15" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - opt (GEN190_1)</t>
         </is>
       </c>
       <c r="H15" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - 9 (GCA282_1)</t>
         </is>
       </c>
       <c r="I15" s="3" t="inlineStr"/>
       <c r="J15" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - 9 (GCA061_1)</t>
         </is>
       </c>
       <c r="K15" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - 9 (GCA259_1)</t>
         </is>
       </c>
       <c r="L15" s="8" t="inlineStr">
@@ -1872,17 +1859,17 @@
       </c>
       <c r="M15" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - opt (GCA316_1)</t>
         </is>
       </c>
       <c r="N15" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - opt (GCA647_1)</t>
         </is>
       </c>
       <c r="O15" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - 9 (GCA282_1)</t>
         </is>
       </c>
       <c r="P15" s="3" t="inlineStr"/>
@@ -1926,17 +1913,17 @@
       </c>
       <c r="C16" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - 5 (GCB058_1)</t>
         </is>
       </c>
       <c r="D16" s="8" t="inlineStr">
         <is>
-          <t>AGRO - opt (GEX431_1)</t>
-        </is>
-      </c>
-      <c r="E16" s="8" t="inlineStr">
-        <is>
-          <t>AGRO - 8 (GCS073_1)</t>
+          <t>AGRO - 5 (GEN081_1)</t>
+        </is>
+      </c>
+      <c r="E16" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AGRO - 5 (GCA238_1) | AGRO - 5 (GCB140_1) </t>
         </is>
       </c>
       <c r="F16" s="8" t="inlineStr">
@@ -1944,9 +1931,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="G16" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">AGRO - 2 (GEX190_1 - GEX190_2) </t>
+      <c r="G16" s="8" t="inlineStr">
+        <is>
+          <t>AGRO - opt (GCA657_1)</t>
         </is>
       </c>
       <c r="H16" s="8" t="inlineStr">
@@ -1955,29 +1942,29 @@
         </is>
       </c>
       <c r="I16" s="3" t="inlineStr"/>
-      <c r="J16" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">AGRO - 4 (GEX116_1 - GEX116_2) </t>
+      <c r="J16" s="8" t="inlineStr">
+        <is>
+          <t>AGRO - 5 (GCA039_1)</t>
         </is>
       </c>
       <c r="K16" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - 5 (GCA038_1)</t>
         </is>
       </c>
       <c r="L16" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - 5 (GCB052_1)</t>
         </is>
       </c>
       <c r="M16" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - opt (GCA646_1)</t>
         </is>
       </c>
       <c r="N16" s="8" t="inlineStr">
         <is>
-          <t>AGRO - 2 (GEX179_1)</t>
+          <t>AGRO - opt (GCA653_1)</t>
         </is>
       </c>
       <c r="O16" s="8" t="inlineStr">
@@ -2029,19 +2016,19 @@
           <t>-</t>
         </is>
       </c>
-      <c r="D17" s="8" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E17" s="8" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="D17" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AGRO - 7 (GCA225_1) | AGRO - 7 (GCA041_1) </t>
+        </is>
+      </c>
+      <c r="E17" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AGRO - 7 (GCA225_1) | AGRO - 7 (GCS247_1) </t>
         </is>
       </c>
       <c r="F17" s="8" t="inlineStr">
         <is>
-          <t>AGRO - 6 (GEX080_1)</t>
+          <t>MED - 6 (GSA197_1)</t>
         </is>
       </c>
       <c r="G17" s="8" t="inlineStr">
@@ -2057,38 +2044,38 @@
       <c r="I17" s="3" t="inlineStr"/>
       <c r="J17" s="8" t="inlineStr">
         <is>
-          <t>AGRO - 6 (GCS243_1)</t>
+          <t>MED - 6 (GSA196_1)</t>
         </is>
       </c>
       <c r="K17" s="8" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L17" s="8" t="inlineStr">
-        <is>
-          <t>-</t>
+          <t>AGRO - 7 (GEN090_1)</t>
+        </is>
+      </c>
+      <c r="L17" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MED - 6 (GSA285_1 -  GSA286_1) </t>
         </is>
       </c>
       <c r="M17" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - 7 (GCA252_1)</t>
         </is>
       </c>
       <c r="N17" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MED - 6 (GSA197_1)</t>
         </is>
       </c>
       <c r="O17" s="8" t="inlineStr">
         <is>
-          <t>CS - 9 (GCH176_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="P17" s="3" t="inlineStr"/>
-      <c r="Q17" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">CS - 2 (GCH1325_1 - GLA102_1) </t>
+      <c r="Q17" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="R17" s="8" t="inlineStr">
@@ -2096,9 +2083,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="S17" s="11" t="inlineStr">
-        <is>
-          <t>CS - 4 + FIL - 4 + MAT - 4 (GCH838_1)</t>
+      <c r="S17" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="T17" s="8" t="inlineStr">
@@ -2108,12 +2095,12 @@
       </c>
       <c r="U17" s="8" t="inlineStr">
         <is>
-          <t>CS - 2 (GCH292_9)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="V17" s="8" t="inlineStr">
         <is>
-          <t>CS - 9 (GCH176_1)</t>
+          <t>-</t>
         </is>
       </c>
     </row>
@@ -2126,12 +2113,12 @@
       </c>
       <c r="C18" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - 6 (GCA231_1)</t>
         </is>
       </c>
       <c r="D18" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - 3 (GCA0683_2)</t>
         </is>
       </c>
       <c r="E18" s="8" t="inlineStr">
@@ -2139,9 +2126,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="F18" s="8" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="F18" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AGRO - 7 (GCS091_1) | AGRO - 7 (GCA287_1) </t>
         </is>
       </c>
       <c r="G18" s="8" t="inlineStr">
@@ -2157,7 +2144,7 @@
       <c r="I18" s="3" t="inlineStr"/>
       <c r="J18" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - 7 (GCA244_1)</t>
         </is>
       </c>
       <c r="K18" s="8" t="inlineStr">
@@ -2167,7 +2154,7 @@
       </c>
       <c r="L18" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - 3 (GEX1047_1)</t>
         </is>
       </c>
       <c r="M18" s="8" t="inlineStr">
@@ -2224,71 +2211,71 @@
           <t>305-A</t>
         </is>
       </c>
-      <c r="C19" s="8" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D19" s="8" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E19" s="8" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F19" s="8" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="C19" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AGRO - 3 (GCA0685_1) | AGRO - 10 (GCA283_1) </t>
+        </is>
+      </c>
+      <c r="D19" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AGRO - 3 (GCA0683_1) | AGRO - 10 (GCA283_1)  | MED - 8 (GSA298_1) </t>
+        </is>
+      </c>
+      <c r="E19" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AGRO - 3 (GCA0683_1) | AGRO - 10 (GCA283_1) </t>
+        </is>
+      </c>
+      <c r="F19" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AGRO - 3 (GCB0607_1) | AGRO - 3 (GCB0608_1)  | AGRO - 10 (GCA283_1) </t>
         </is>
       </c>
       <c r="G19" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - 10 (GCA283_1)</t>
         </is>
       </c>
       <c r="H19" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - 10 (GCA283_1)</t>
         </is>
       </c>
       <c r="I19" s="3" t="inlineStr"/>
       <c r="J19" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MED - 8 (GSA291_1)</t>
         </is>
       </c>
       <c r="K19" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MED - 8 (GSA298_1)</t>
         </is>
       </c>
       <c r="L19" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MED - 8 (GSA289_1)</t>
         </is>
       </c>
       <c r="M19" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MED - 8 (GSA290_1)</t>
         </is>
       </c>
       <c r="N19" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MED - 8 (GSA289_1)</t>
         </is>
       </c>
       <c r="O19" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - 10 (GCA283_1)</t>
         </is>
       </c>
       <c r="P19" s="3" t="inlineStr"/>
       <c r="Q19" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MED - 8 (GSA291_1)</t>
         </is>
       </c>
       <c r="R19" s="8" t="inlineStr">
@@ -2303,17 +2290,17 @@
       </c>
       <c r="T19" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MED - 8 (GSA290_1)</t>
         </is>
       </c>
       <c r="U19" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - 10 (GCA283_1)</t>
         </is>
       </c>
       <c r="V19" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AGRO - 10 (GCA283_1)</t>
         </is>
       </c>
     </row>
@@ -2331,7 +2318,7 @@
       </c>
       <c r="D20" s="8" t="inlineStr">
         <is>
-          <t>ENF - 10 (GSA049_1)</t>
+          <t>AGRO - 3 (GCB057_1)</t>
         </is>
       </c>
       <c r="E20" s="8" t="inlineStr">
@@ -2357,27 +2344,27 @@
       <c r="I20" s="3" t="inlineStr"/>
       <c r="J20" s="8" t="inlineStr">
         <is>
-          <t>ENF - 10 (GSA047_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="K20" s="8" t="inlineStr">
         <is>
-          <t>ENF - 10 (GSA047_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="L20" s="8" t="inlineStr">
         <is>
-          <t>ENF - 10 (GSA047_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M20" s="8" t="inlineStr">
         <is>
-          <t>ENF - 10 (GSA047_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="N20" s="8" t="inlineStr">
         <is>
-          <t>ENF - 10 (GSA047_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="O20" s="8" t="inlineStr">
@@ -2386,19 +2373,19 @@
         </is>
       </c>
       <c r="P20" s="3" t="inlineStr"/>
-      <c r="Q20" s="11" t="inlineStr">
-        <is>
-          <t>CS - 8 + HIS - 4 (GCS238_5)</t>
+      <c r="Q20" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="R20" s="8" t="inlineStr">
         <is>
-          <t>HIS - 7 (GLA108_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="S20" s="8" t="inlineStr">
         <is>
-          <t>HIS - opt (GCH467_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="T20" s="8" t="inlineStr">
@@ -2431,7 +2418,7 @@
       </c>
       <c r="D21" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MED - 8 (GSA298_1)</t>
         </is>
       </c>
       <c r="E21" s="8" t="inlineStr">
@@ -2441,7 +2428,7 @@
       </c>
       <c r="F21" s="8" t="inlineStr">
         <is>
-          <t>HIS - 8 (GCH390_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G21" s="8" t="inlineStr">
@@ -2462,7 +2449,7 @@
       </c>
       <c r="K21" s="8" t="inlineStr">
         <is>
-          <t>ENF - 6 (GSA044_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="L21" s="8" t="inlineStr">
@@ -2472,7 +2459,7 @@
       </c>
       <c r="M21" s="8" t="inlineStr">
         <is>
-          <t>ENF - 6 (GSA044_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="N21" s="8" t="inlineStr">
@@ -2488,7 +2475,7 @@
       <c r="P21" s="3" t="inlineStr"/>
       <c r="Q21" s="8" t="inlineStr">
         <is>
-          <t>HIS - 8 (GCH389_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="R21" s="8" t="inlineStr">
@@ -2498,17 +2485,17 @@
       </c>
       <c r="S21" s="8" t="inlineStr">
         <is>
-          <t>HIS - opt (GCH459_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="T21" s="8" t="inlineStr">
         <is>
-          <t>HIS - 8 (GCH390_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U21" s="8" t="inlineStr">
         <is>
-          <t>HIS - 8 (GCH388_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="V21" s="8" t="inlineStr">
@@ -2526,22 +2513,22 @@
       </c>
       <c r="C22" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ENF - 3 (GCS011_1)</t>
         </is>
       </c>
       <c r="D22" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ENF - 1 (GCH029_1)</t>
         </is>
       </c>
       <c r="E22" s="8" t="inlineStr">
         <is>
-          <t>ENF - 2 (GSA0304_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F22" s="8" t="inlineStr">
         <is>
-          <t>ENF - 2 (GSA0305_1)</t>
+          <t>ENF - opt (GSA0307_1)</t>
         </is>
       </c>
       <c r="G22" s="8" t="inlineStr">
@@ -2557,7 +2544,7 @@
       <c r="I22" s="3" t="inlineStr"/>
       <c r="J22" s="8" t="inlineStr">
         <is>
-          <t>ENF - 2 (GCB064_1)</t>
+          <t>ENF - 1 (GLA001_1)</t>
         </is>
       </c>
       <c r="K22" s="8" t="inlineStr">
@@ -2572,12 +2559,12 @@
       </c>
       <c r="M22" s="8" t="inlineStr">
         <is>
-          <t>ENF - 2 (GCB019_1)</t>
+          <t>ENF - 3 (GCS010_1)</t>
         </is>
       </c>
       <c r="N22" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ENF - opt (GSA0307_1)</t>
         </is>
       </c>
       <c r="O22" s="8" t="inlineStr">
@@ -2588,22 +2575,22 @@
       <c r="P22" s="3" t="inlineStr"/>
       <c r="Q22" s="8" t="inlineStr">
         <is>
-          <t>HIS - 2 (GCH290_15)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="R22" s="8" t="inlineStr">
         <is>
-          <t>HIS - 2 (GCH291_3)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="S22" s="8" t="inlineStr">
         <is>
-          <t>HIS - 2 (GCH366_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="T22" s="8" t="inlineStr">
         <is>
-          <t>HIS - 2 (GCH365_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U22" s="8" t="inlineStr">
@@ -2626,22 +2613,22 @@
       </c>
       <c r="C23" s="8" t="inlineStr">
         <is>
-          <t>ENF - 4 (GCB064_2)</t>
+          <t>ENF - 5 (GSA018_1)</t>
         </is>
       </c>
       <c r="D23" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ENF - 5 (GSA019_1)</t>
         </is>
       </c>
       <c r="E23" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ENF - 5 (GSA018_1)</t>
         </is>
       </c>
       <c r="F23" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ENF - 5 (GSA018_1)</t>
         </is>
       </c>
       <c r="G23" s="8" t="inlineStr">
@@ -2657,27 +2644,27 @@
       <c r="I23" s="3" t="inlineStr"/>
       <c r="J23" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ENF - 5 (GCB080_1)</t>
         </is>
       </c>
       <c r="K23" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ENF - 5 (GSA020_1)</t>
         </is>
       </c>
       <c r="L23" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ENF - 5 (GSA019_1)</t>
         </is>
       </c>
       <c r="M23" s="8" t="inlineStr">
         <is>
-          <t>ENF - 4 (GCB029_1)</t>
+          <t>ENF - 5 (GSA019_1)</t>
         </is>
       </c>
       <c r="N23" s="8" t="inlineStr">
         <is>
-          <t>ENF - 4 (GCB019_2)</t>
+          <t>ENF - 5 (GSA018_1)</t>
         </is>
       </c>
       <c r="O23" s="8" t="inlineStr">
@@ -2703,7 +2690,7 @@
       </c>
       <c r="T23" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>HIS - 3 (GCH369_1)</t>
         </is>
       </c>
       <c r="U23" s="8" t="inlineStr">
@@ -3316,7 +3303,7 @@
       <c r="P30" s="3" t="inlineStr"/>
       <c r="Q30" s="8" t="inlineStr">
         <is>
-          <t>PED - 1 (GCH1036_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="R30" s="8" t="inlineStr">
@@ -3331,7 +3318,7 @@
       </c>
       <c r="T30" s="8" t="inlineStr">
         <is>
-          <t>PED - 1 (GCH1035_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U30" s="8" t="inlineStr">
@@ -3354,7 +3341,7 @@
       </c>
       <c r="C31" s="8" t="inlineStr">
         <is>
-          <t>PED - 6 (GLA239_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D31" s="8" t="inlineStr">
@@ -3364,7 +3351,7 @@
       </c>
       <c r="E31" s="8" t="inlineStr">
         <is>
-          <t>PED - 6 (GLA238_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F31" s="8" t="inlineStr">
@@ -3416,12 +3403,12 @@
       <c r="P31" s="3" t="inlineStr"/>
       <c r="Q31" s="8" t="inlineStr">
         <is>
-          <t>PED - 3 (GCH1086_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="R31" s="8" t="inlineStr">
         <is>
-          <t>PED - 3 (GCH1087_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="S31" s="8" t="inlineStr">
@@ -3431,12 +3418,12 @@
       </c>
       <c r="T31" s="8" t="inlineStr">
         <is>
-          <t>PED - 9 (GCH1280_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U31" s="8" t="inlineStr">
         <is>
-          <t>PED - 3 (GCH1088_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="V31" s="8" t="inlineStr">
@@ -3464,7 +3451,7 @@
       </c>
       <c r="E32" s="8" t="inlineStr">
         <is>
-          <t>PED - opt (GCH1302_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F32" s="8" t="inlineStr">
@@ -3516,7 +3503,7 @@
       <c r="P32" s="3" t="inlineStr"/>
       <c r="Q32" s="8" t="inlineStr">
         <is>
-          <t>PED - 5 (GLA237_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="R32" s="8" t="inlineStr">
@@ -3526,17 +3513,17 @@
       </c>
       <c r="S32" s="8" t="inlineStr">
         <is>
-          <t>PED - opt (GCH1301_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="T32" s="8" t="inlineStr">
         <is>
-          <t>PED - opt (GCH1286_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U32" s="8" t="inlineStr">
         <is>
-          <t>PED - opt (GCH1284_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="V32" s="8" t="inlineStr">
@@ -3554,27 +3541,27 @@
       </c>
       <c r="C33" s="8" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D33" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">PED - 2 (GCH1038_1 - GCH1039_1) </t>
+          <t>PED - 7 (GCH1120_1)</t>
+        </is>
+      </c>
+      <c r="D33" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="E33" s="8" t="inlineStr">
         <is>
-          <t>PED - 2 (GCH1037_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F33" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>PED - 7 (GLA240_1)</t>
         </is>
       </c>
       <c r="G33" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>PED - 7 (GEX776_1)</t>
         </is>
       </c>
       <c r="H33" s="8" t="inlineStr">
@@ -3616,12 +3603,12 @@
       <c r="P33" s="3" t="inlineStr"/>
       <c r="Q33" s="8" t="inlineStr">
         <is>
-          <t>PED - 7 (GLA213_1)</t>
+          <t>PED - 7 (GCH162_1)</t>
         </is>
       </c>
       <c r="R33" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>PED - 8 (GCH1123_1)</t>
         </is>
       </c>
       <c r="S33" s="8" t="inlineStr">
@@ -3631,12 +3618,12 @@
       </c>
       <c r="T33" s="8" t="inlineStr">
         <is>
-          <t>PED - 7 (GLA240_1)</t>
+          <t>PED - 8 (GCH1124_1)</t>
         </is>
       </c>
       <c r="U33" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>PED - 8 (GCH1125_1)</t>
         </is>
       </c>
       <c r="V33" s="8" t="inlineStr">
@@ -3659,12 +3646,12 @@
       </c>
       <c r="D34" s="8" t="inlineStr">
         <is>
-          <t>ADM - 6 (GCS541_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E34" s="8" t="inlineStr">
         <is>
-          <t>ADM - 6 (GCS543_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F34" s="8" t="inlineStr">
@@ -3674,7 +3661,7 @@
       </c>
       <c r="G34" s="8" t="inlineStr">
         <is>
-          <t>ADM - 6 (GCS542_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H34" s="8" t="inlineStr">
@@ -3726,12 +3713,12 @@
       </c>
       <c r="S34" s="8" t="inlineStr">
         <is>
-          <t>ADM - 7 (GCS544_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="T34" s="8" t="inlineStr">
         <is>
-          <t>ADM - 7 (GCS545_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U34" s="8" t="inlineStr">
@@ -3759,12 +3746,12 @@
       </c>
       <c r="D35" s="8" t="inlineStr">
         <is>
-          <t>ADM - 8 (GCS546_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E35" s="8" t="inlineStr">
         <is>
-          <t>ADM - 8 (GCS548_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F35" s="8" t="inlineStr">
@@ -3774,7 +3761,7 @@
       </c>
       <c r="G35" s="8" t="inlineStr">
         <is>
-          <t>ADM - 8 (GCS547_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H35" s="8" t="inlineStr">
@@ -3821,7 +3808,7 @@
       </c>
       <c r="R35" s="8" t="inlineStr">
         <is>
-          <t>ADM - 9 (GCS549_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="S35" s="8" t="inlineStr">
@@ -3854,17 +3841,17 @@
       </c>
       <c r="C36" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ADM - 9 (GCS550_1)</t>
         </is>
       </c>
       <c r="D36" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ADM - 9 (GCS551_1)</t>
         </is>
       </c>
       <c r="E36" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ADM - 9 (GCS573_1)</t>
         </is>
       </c>
       <c r="F36" s="8" t="inlineStr">
@@ -3926,7 +3913,7 @@
       </c>
       <c r="S36" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ADM - opt (GCS555_1)</t>
         </is>
       </c>
       <c r="T36" s="8" t="inlineStr">
@@ -4179,23 +4166,23 @@
       </c>
       <c r="H39" s="8" t="inlineStr">
         <is>
-          <t>GEO - 4 (GEX559_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I39" s="3" t="inlineStr"/>
-      <c r="J39" s="8" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="J39" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CC - 3 (GEX098_1) | CC - 7 (GEX395_1) </t>
         </is>
       </c>
       <c r="K39" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>CC - 3 (GEX098_1)</t>
         </is>
       </c>
       <c r="L39" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>CC - 7 (GEX395_1)</t>
         </is>
       </c>
       <c r="M39" s="8" t="inlineStr">
@@ -4216,27 +4203,27 @@
       <c r="P39" s="3" t="inlineStr"/>
       <c r="Q39" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>CC - 4 (GEX615_1)</t>
         </is>
       </c>
       <c r="R39" s="8" t="inlineStr">
         <is>
-          <t>GEO - 4 (GEX559_1)</t>
+          <t>CC - 4 (GEX613_1)</t>
         </is>
       </c>
       <c r="S39" s="8" t="inlineStr">
         <is>
-          <t>GEO - 2 (GCH290_8)</t>
+          <t>CC - 4 (GEX612_1)</t>
         </is>
       </c>
       <c r="T39" s="8" t="inlineStr">
         <is>
-          <t>GEO - 8 (GCH292_10)</t>
+          <t>CC - 4 (GEX090_1)</t>
         </is>
       </c>
       <c r="U39" s="8" t="inlineStr">
         <is>
-          <t>GEO - 4 (GCH293_6)</t>
+          <t>CC - 4 (GEX195_1)</t>
         </is>
       </c>
       <c r="V39" s="8" t="inlineStr">
@@ -4254,12 +4241,12 @@
       </c>
       <c r="C40" s="8" t="inlineStr">
         <is>
-          <t>MED - 1 (GSA271_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D40" s="8" t="inlineStr">
         <is>
-          <t>MED - 1 (GSA271_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E40" s="8" t="inlineStr">
@@ -4269,12 +4256,12 @@
       </c>
       <c r="F40" s="8" t="inlineStr">
         <is>
-          <t>MED - 1 (GCH290_13)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G40" s="8" t="inlineStr">
         <is>
-          <t>MED - 1 (GSA271_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H40" s="8" t="inlineStr">
@@ -4283,29 +4270,29 @@
         </is>
       </c>
       <c r="I40" s="3" t="inlineStr"/>
-      <c r="J40" s="9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">MED - 1 (GCH293_8) | MED - opt (GSA299_1) </t>
+      <c r="J40" s="8" t="inlineStr">
+        <is>
+          <t>CC - 3 (GEX098_2)</t>
         </is>
       </c>
       <c r="K40" s="8" t="inlineStr">
         <is>
-          <t>MED - 5 (GSA284_1)</t>
+          <t>CC - 3 (GEX098_2)</t>
         </is>
       </c>
       <c r="L40" s="8" t="inlineStr">
         <is>
-          <t>MED - 1 (GSA271_1)</t>
+          <t>CC - 7 (GCS238_1)</t>
         </is>
       </c>
       <c r="M40" s="8" t="inlineStr">
         <is>
-          <t>MED - 5 (GSA283_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="N40" s="8" t="inlineStr">
         <is>
-          <t>MED - 1 (GSA268_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="O40" s="8" t="inlineStr">
@@ -4316,27 +4303,27 @@
       <c r="P40" s="3" t="inlineStr"/>
       <c r="Q40" s="8" t="inlineStr">
         <is>
-          <t>MED - opt (GSA299_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="R40" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>CC - 4 (GEX613_2)</t>
         </is>
       </c>
       <c r="S40" s="8" t="inlineStr">
         <is>
-          <t>MED - opt (GLA192_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="T40" s="8" t="inlineStr">
         <is>
-          <t>MED - 5 (GSA283_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U40" s="8" t="inlineStr">
         <is>
-          <t>MED - 1 (GLA104_8)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="V40" s="8" t="inlineStr">
@@ -4359,17 +4346,17 @@
       </c>
       <c r="D41" s="8" t="inlineStr">
         <is>
-          <t>MED - 3 (GSA280_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E41" s="8" t="inlineStr">
         <is>
-          <t>MED - 7 (GSA287_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F41" s="8" t="inlineStr">
         <is>
-          <t>MED - 7 (GCS239_11)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G41" s="8" t="inlineStr">
@@ -4385,27 +4372,27 @@
       <c r="I41" s="3" t="inlineStr"/>
       <c r="J41" s="9" t="inlineStr">
         <is>
-          <t xml:space="preserve">MED - 3 (GSA280_1) | MED - 9 (GSA296_1) </t>
-        </is>
-      </c>
-      <c r="K41" s="8" t="inlineStr">
-        <is>
-          <t>MED - 3 (GSA280_1)</t>
-        </is>
-      </c>
-      <c r="L41" s="8" t="inlineStr">
-        <is>
-          <t>-</t>
+          <t xml:space="preserve">CC - 1 (GEX003_1) | CC - 1 (GEX208_1) </t>
+        </is>
+      </c>
+      <c r="K41" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CC - 1 (GEX003_1) | CC - 1 (GEX208_1) </t>
+        </is>
+      </c>
+      <c r="L41" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CC - 1 (GEX210_1) | CC - 1 (GCH293_1) </t>
         </is>
       </c>
       <c r="M41" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>CC - 1 (GEX210_1)</t>
         </is>
       </c>
       <c r="N41" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>CC - 1 (GCH293_1)</t>
         </is>
       </c>
       <c r="O41" s="8" t="inlineStr">
@@ -4416,7 +4403,7 @@
       <c r="P41" s="3" t="inlineStr"/>
       <c r="Q41" s="8" t="inlineStr">
         <is>
-          <t>MED - 9 (GSA296_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="R41" s="8" t="inlineStr">
@@ -4431,7 +4418,7 @@
       </c>
       <c r="T41" s="8" t="inlineStr">
         <is>
-          <t>MED - 3 (GSA281_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U41" s="8" t="inlineStr">
@@ -4469,43 +4456,43 @@
       </c>
       <c r="F42" s="8" t="inlineStr">
         <is>
-          <t>CC - 8 (GEX658_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G42" s="8" t="inlineStr">
         <is>
-          <t>CC - 8 (GEX658_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H42" s="8" t="inlineStr">
         <is>
-          <t>CC - 8 (GEX658_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I42" s="3" t="inlineStr"/>
-      <c r="J42" s="8" t="inlineStr">
-        <is>
-          <t>CC - 8 (GCS239_2)</t>
+      <c r="J42" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CC - 1 (GEX003_2) | CC - 1 (GEX208_2) </t>
         </is>
       </c>
       <c r="K42" s="9" t="inlineStr">
         <is>
-          <t xml:space="preserve">CC - 6 (GCS580_1) | CC - 6 (GEX614_1) </t>
+          <t xml:space="preserve">CC - 1 (GEX003_2) | CC - 1 (GEX208_2) </t>
         </is>
       </c>
       <c r="L42" s="8" t="inlineStr">
         <is>
-          <t>CC - 6 (GCH292_2)</t>
+          <t>CC - opt (GEX1087_1)</t>
         </is>
       </c>
       <c r="M42" s="8" t="inlineStr">
         <is>
-          <t>CC - 6 (GCS580_1)</t>
+          <t>CC - opt (GEX1087_1)</t>
         </is>
       </c>
       <c r="N42" s="8" t="inlineStr">
         <is>
-          <t>CC - 6 (GEX614_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="O42" s="8" t="inlineStr">
@@ -4516,17 +4503,17 @@
       <c r="P42" s="3" t="inlineStr"/>
       <c r="Q42" s="8" t="inlineStr">
         <is>
-          <t>CC - opt (GEX635_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="R42" s="8" t="inlineStr">
         <is>
-          <t>CC - 7 (GCS238_2)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="S42" s="8" t="inlineStr">
         <is>
-          <t>CC - 7 (GEX618_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="T42" s="8" t="inlineStr">
@@ -4536,7 +4523,7 @@
       </c>
       <c r="U42" s="8" t="inlineStr">
         <is>
-          <t>CC - 7 (GEX617_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="V42" s="8" t="inlineStr">
@@ -4569,23 +4556,23 @@
       </c>
       <c r="F43" s="8" t="inlineStr">
         <is>
-          <t>CC - 9 (GEX657_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G43" s="8" t="inlineStr">
         <is>
-          <t>CC - 9 (GEX657_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H43" s="8" t="inlineStr">
         <is>
-          <t>CC - 9 (GEX657_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I43" s="3" t="inlineStr"/>
       <c r="J43" s="8" t="inlineStr">
         <is>
-          <t>CC - 4 (GEX613_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="K43" s="8" t="inlineStr">
@@ -4605,7 +4592,7 @@
       </c>
       <c r="N43" s="8" t="inlineStr">
         <is>
-          <t>CC - 4 (GEX613_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="O43" s="8" t="inlineStr">
@@ -4626,7 +4613,7 @@
       </c>
       <c r="S43" s="8" t="inlineStr">
         <is>
-          <t>CC - 4 (GCH290_5)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="T43" s="8" t="inlineStr">
@@ -4636,7 +4623,7 @@
       </c>
       <c r="U43" s="8" t="inlineStr">
         <is>
-          <t>CC - 5 (GEX616_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="V43" s="8" t="inlineStr">
@@ -4685,27 +4672,27 @@
       <c r="I44" s="3" t="inlineStr"/>
       <c r="J44" s="8" t="inlineStr">
         <is>
-          <t>CC - 4 (GEX613_2)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="K44" s="8" t="inlineStr">
         <is>
-          <t>CC - 4 (GEN254_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="L44" s="8" t="inlineStr">
         <is>
-          <t>CC - 4 (GEX090_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M44" s="8" t="inlineStr">
         <is>
-          <t>CC - 4 (GEN254_1)</t>
-        </is>
-      </c>
-      <c r="N44" s="9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">CC - 4 (GEX090_1) | CC - 4 (GEX613_2) </t>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N44" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="O44" s="8" t="inlineStr">
@@ -4731,7 +4718,7 @@
       </c>
       <c r="T44" s="8" t="inlineStr">
         <is>
-          <t>CC - 1 (GEX003_2)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U44" s="8" t="inlineStr">
@@ -4785,12 +4772,12 @@
       <c r="I45" s="3" t="inlineStr"/>
       <c r="J45" s="8" t="inlineStr">
         <is>
-          <t>CC - 2 (GEN253_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="K45" s="8" t="inlineStr">
         <is>
-          <t>CC - 2 (GEN253_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="L45" s="8" t="inlineStr">
@@ -4800,12 +4787,12 @@
       </c>
       <c r="M45" s="8" t="inlineStr">
         <is>
-          <t>CC - 2 (GEX055_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="N45" s="8" t="inlineStr">
         <is>
-          <t>CC - 2 (GEX055_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="O45" s="8" t="inlineStr">
@@ -4816,7 +4803,7 @@
       <c r="P45" s="3" t="inlineStr"/>
       <c r="Q45" s="8" t="inlineStr">
         <is>
-          <t>CC - 1 (GCH293_2)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="R45" s="8" t="inlineStr">
@@ -4826,12 +4813,12 @@
       </c>
       <c r="S45" s="8" t="inlineStr">
         <is>
-          <t>CC - 2 (GLA104_2)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="T45" s="8" t="inlineStr">
         <is>
-          <t>CC - 1 (GEX003_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U45" s="8" t="inlineStr">
@@ -5318,7 +5305,7 @@
       </c>
       <c r="K51" s="8" t="inlineStr">
         <is>
-          <t>FIL - 6 (GCH837_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="L51" s="8" t="inlineStr">
@@ -5338,23 +5325,23 @@
       </c>
       <c r="O51" s="8" t="inlineStr">
         <is>
-          <t>FIL - 8 (GCH843_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="P51" s="3" t="inlineStr"/>
       <c r="Q51" s="8" t="inlineStr">
         <is>
-          <t>FIL - 6 (GCH839_2)</t>
+          <t>FIL - 2 (GCH855_1)</t>
         </is>
       </c>
       <c r="R51" s="8" t="inlineStr">
         <is>
-          <t>FIL - 6 (GCH837_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="S51" s="8" t="inlineStr">
         <is>
-          <t>FIL - 8 (GCH844_1)</t>
+          <t>FIL - opt (GCH892_1)</t>
         </is>
       </c>
       <c r="T51" s="8" t="inlineStr">
@@ -5428,7 +5415,7 @@
       </c>
       <c r="M52" s="8" t="inlineStr">
         <is>
-          <t>FIL - 2 (GCH845_1)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="N52" s="8" t="inlineStr">
@@ -5444,27 +5431,27 @@
       <c r="P52" s="3" t="inlineStr"/>
       <c r="Q52" s="8" t="inlineStr">
         <is>
-          <t>FIL - 4 (GCH847_1)</t>
+          <t>FIL - 1 (GCH293_2)</t>
         </is>
       </c>
       <c r="R52" s="8" t="inlineStr">
         <is>
-          <t>FIL - 2 (GLA103_3)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="S52" s="8" t="inlineStr">
         <is>
-          <t>FIL - 2 (GEX211_2)</t>
+          <t>FIL - 1 (GCH822_1)</t>
         </is>
       </c>
       <c r="T52" s="8" t="inlineStr">
         <is>
-          <t>FIL - 2 (GCH845_1)</t>
+          <t>FIL - 1 (GCH823_1)</t>
         </is>
       </c>
       <c r="U52" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>FIL - 1 (GCH290_1)</t>
         </is>
       </c>
       <c r="V52" s="8" t="inlineStr">
@@ -5802,7 +5789,7 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="12" t="n"/>
+      <c r="A57" s="11" t="n"/>
       <c r="B57" s="6" t="inlineStr">
         <is>
           <t>110-DE</t>
@@ -5841,27 +5828,27 @@
       <c r="I57" s="3" t="inlineStr"/>
       <c r="J57" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>LET - opt (GLA553_1)</t>
         </is>
       </c>
       <c r="K57" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>LET - opt (GLA553_1)</t>
         </is>
       </c>
       <c r="L57" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>LET - opt (GLA553_1)</t>
         </is>
       </c>
       <c r="M57" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>LET - opt (GLA553_1)</t>
         </is>
       </c>
       <c r="N57" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>LET - opt (GLA553_1)</t>
         </is>
       </c>
       <c r="O57" s="8" t="inlineStr">
@@ -5872,12 +5859,12 @@
       <c r="P57" s="3" t="inlineStr"/>
       <c r="Q57" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>LET - 1 (GCH292_1)</t>
         </is>
       </c>
       <c r="R57" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>LET - 1 (GLA355_1)</t>
         </is>
       </c>
       <c r="S57" s="8" t="inlineStr">
@@ -5887,12 +5874,12 @@
       </c>
       <c r="T57" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>LET - opt (GLA517_1)</t>
         </is>
       </c>
       <c r="U57" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>LET - opt (GLA550_1)</t>
         </is>
       </c>
       <c r="V57" s="8" t="inlineStr">

</xml_diff>